<commit_message>
Added DSA worddoc and updated excel with formatting
</commit_message>
<xml_diff>
--- a/Understanding-Algorithms-for-Interview.xlsx
+++ b/Understanding-Algorithms-for-Interview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachauh\Google Drive\Excell-Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f69pl7i\my-repos\algorithms-and-interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0FD646-2F5E-415D-9B06-E75504F405F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04C69AE-698E-4C51-B2D9-D7A5880ED7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" tabRatio="766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="766" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithms &amp; Contents" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="352">
   <si>
     <t>Chapter</t>
   </si>
@@ -1677,7 +1677,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1687,6 +1687,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1704,16 +1710,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1735,8 +1739,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1767,8 +1809,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>307975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1815,8 +1857,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>307975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2121,34 +2163,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.46484375" customWidth="1"/>
-    <col min="3" max="3" width="27.86328125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>73</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2156,55 +2198,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2.1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2.5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2.6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2212,259 +2254,259 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3.1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3.2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3.4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.7</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>4.2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>4.3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>4.5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4.7</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="203" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>5.2</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>5.3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5.4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>5.6</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5.7</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5.8</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>5.9</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>6.1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6.2</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>6.3</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>6.4</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>6.5</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2472,263 +2514,263 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>7.1</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="6" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>7.2</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>7.3</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>7.4</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>7.5</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>7.6</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>8</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="6" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>8.1</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>8.4</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>9.1</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>9.4</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>9.5</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>10</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>10.1</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>10.199999999999999</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>10.3</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>10.4</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>11</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="6" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>11.1</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>11.2</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>11.3</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>11.4</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>11.5</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>11.6</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>12</v>
       </c>
@@ -2736,36 +2778,36 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>12.1</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C72" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C72" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C73" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C73" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C74" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C74" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C75" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C75" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C76" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C76" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2780,96 +2822,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CC528E-249D-4357-BFE7-93734FE7C3C3}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="7"/>
-    <col min="4" max="4" width="37.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="32.9296875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="5.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" style="5"/>
+    <col min="4" max="4" width="15.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D8" s="7" t="s">
+    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="D8" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D9" s="7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D9" s="5" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2884,12 +2929,12 @@
   <dimension ref="B2:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>179</v>
       </c>
@@ -2897,7 +2942,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>181</v>
       </c>
@@ -2909,132 +2954,130 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B537A8-1C1F-4F9E-BB39-AB3C7132CBBB}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="60.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="6.9296875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="49.59765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="49.6328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C6" s="13" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C7" s="13" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C8" s="13" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C12" s="12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C14" s="7" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" s="5" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" s="5" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3049,59 +3092,59 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.9296875" customWidth="1"/>
-    <col min="2" max="2" width="76" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="52" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3114,53 +3157,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1778B0E5-64C4-4AFF-94CB-48F121A59C9D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="19" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="93.6640625" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="17" t="s">
         <v>350</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="16" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D3" t="s">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D3" s="6" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>349</v>
       </c>
     </row>
@@ -3172,49 +3215,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FC6FBE-4FB7-424C-AF12-04CD0C8E5C40}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="90.1328125" customWidth="1"/>
+    <col min="3" max="3" width="58.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="4" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3229,302 +3281,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF8BC6A-B4FA-41B4-BBA4-5757332229B9}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.46484375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="77.19921875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13" style="5" customWidth="1"/>
+    <col min="3" max="3" width="58.81640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="7">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="7">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C5" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C6" s="7" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="7">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C10" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C11" s="6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C12" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="7">
+    <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="7">
+    <row r="16" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="7">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
         <v>3</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="7">
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
         <v>5</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="7">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
         <v>6</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C21" s="7" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C21" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C24" s="7" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B26" s="11" t="s">
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C27" s="7" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C27" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C28" s="7" t="s">
+    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C28" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C30" s="7" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C30" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C31" s="7" t="s">
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C31" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C34" s="7" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C34" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C35" s="7" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C35" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C36" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="8" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="7">
+    <row r="38" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="5">
         <v>1</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B39" s="11"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="7">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="5">
         <v>2</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D41" s="5" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D42" s="5" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D43" s="5" t="s">
         <v>344</v>
       </c>
     </row>
@@ -3539,115 +3591,115 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="5" max="5" width="75.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="59.08984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>265</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>263</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C4" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C5" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E11" t="s">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E11" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E14" t="s">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E14" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>177</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="E18" t="s">
+    <row r="18" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E18" s="4" t="s">
         <v>268</v>
       </c>
     </row>
@@ -3662,128 +3714,167 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.9296875" customWidth="1"/>
-    <col min="3" max="3" width="59.19921875" customWidth="1"/>
-    <col min="4" max="4" width="21.46484375" customWidth="1"/>
-    <col min="5" max="5" width="25.59765625" customWidth="1"/>
-    <col min="7" max="7" width="0.9296875" customWidth="1"/>
-    <col min="8" max="8" width="7.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" customWidth="1"/>
+    <col min="3" max="3" width="46.1796875" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" customWidth="1"/>
+    <col min="7" max="7" width="0.90625" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I5" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I7" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
         <v>228</v>
       </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3793,227 +3884,248 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8C5570-2255-4986-BF37-942D756859F6}">
-  <dimension ref="A2:N42"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.53125" customWidth="1"/>
-    <col min="4" max="4" width="76.86328125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="19.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="48" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="B2" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D4" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D10" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D13" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D16" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D18" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D19" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D20" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D21" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D22" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D23" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B24" s="13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="N30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D31" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="D32" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="5"/>
+      <c r="D35" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="5"/>
+      <c r="D36" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="5"/>
+      <c r="D37" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
+    <row r="38" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="B38" s="5"/>
+      <c r="D38" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+    <row r="39" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39" s="5"/>
+      <c r="D39" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="5"/>
+      <c r="D41" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+    <row r="42" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="5"/>
+      <c r="D42" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B11" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D27" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B33" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" t="s">
-        <v>166</v>
-      </c>
-      <c r="N39" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="D40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="D41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B42" t="s">
-        <v>170</v>
-      </c>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4023,190 +4135,191 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F506C32F-6417-48D3-881C-7E8516D3350A}">
-  <dimension ref="B1:E37"/>
+  <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection sqref="A1:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.19921875" customWidth="1"/>
-    <col min="4" max="4" width="84.9296875" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
+    <row r="1" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="25" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="3" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
+    <row r="4" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D5" t="s">
+    <row r="5" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C5" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+    <row r="6" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+    <row r="7" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="C7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
+    <row r="8" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="C8" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C14" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
+    <row r="15" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="C15" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C16" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C17" t="s">
+    <row r="17" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C17" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C18" t="s">
+    <row r="18" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C18" s="6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C19" t="s">
+    <row r="19" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C19" s="6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C20" t="s">
+    <row r="20" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="C20" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C21" t="s">
+    <row r="21" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C21" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C22" t="s">
+    <row r="22" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C22" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C23" t="s">
+    <row r="23" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C23" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C25" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C27" t="s">
+    <row r="27" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C27" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
+    <row r="29" spans="2:4" ht="174" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
+    <row r="31" spans="2:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="6" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
+    <row r="33" spans="2:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="6" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
+    <row r="35" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D36" t="s">
+    <row r="36" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="D36" s="6" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D37" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D37" s="5" t="s">
         <v>317</v>
       </c>
     </row>
@@ -4221,71 +4334,77 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B34B052-5D1F-46CC-9770-329FC11CE19F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" customWidth="1"/>
-    <col min="3" max="3" width="12.265625" customWidth="1"/>
-    <col min="6" max="6" width="63.19921875" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="45.54296875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
+    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="F7" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>